<commit_message>
Inicio de programación para aceptar archivos .csv y .xlsx
</commit_message>
<xml_diff>
--- a/experimentacion.xlsx
+++ b/experimentacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - INEGI\Desktop\Documentos\R\Cursos\Topicos_R_otono_2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - INEGI\Desktop\Documentos\R\Cursos\Topicos_R_otono_2021\shiny_box_plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="20" documentId="8_{28B71D1B-D2AA-4460-A95F-CEA9FDD18E81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{607AF968-E529-411A-B90B-F5FD061AB064}"/>
@@ -746,9 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2740D4DB-16E5-4610-A881-32A6DD2AD235}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2252,6 +2250,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008AA28B37E4B0C488BC610126A1D2958" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb1ab38a74b58b4200af173ddb48f706">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c59651c7-6227-4868-bf59-399a3b5e34f6" xmlns:ns4="17389ab1-7684-4b99-b6a5-557e8d0dcb1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="22df3d62d6dc641b2398017aaf99ba40" ns3:_="" ns4:_="">
     <xsd:import namespace="c59651c7-6227-4868-bf59-399a3b5e34f6"/>
@@ -2474,12 +2478,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2490,6 +2488,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC1185DE-0B7F-4004-876A-BABDC946D68C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="17389ab1-7684-4b99-b6a5-557e8d0dcb1b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c59651c7-6227-4868-bf59-399a3b5e34f6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C40E00-A685-447E-8902-9742E1F8D651}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2508,23 +2523,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC1185DE-0B7F-4004-876A-BABDC946D68C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="17389ab1-7684-4b99-b6a5-557e8d0dcb1b"/>
-    <ds:schemaRef ds:uri="c59651c7-6227-4868-bf59-399a3b5e34f6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA5140BD-86DF-4EBF-854E-7EC02927E757}">
   <ds:schemaRefs>

</xml_diff>